<commit_message>
removed particleData tests, will be needed later
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>count</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>vector&lt;ptr&lt;Obj&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Obj SoA</t>
   </si>
   <si>
     <t>updates</t>
@@ -44,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -85,7 +82,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -335,114 +332,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Obj SoA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$B$4:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>21000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$E$4:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0" formatCode="0.0000">
-                  <c:v>12.704599999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>51.326300000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>115.51300000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>205.19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>320.32400000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>461.291</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>626.66600000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>818.22900000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1034.8599999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1276.76</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1542.46</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="80989568"/>
-        <c:axId val="58179584"/>
+        <c:axId val="65725952"/>
+        <c:axId val="66265088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80989568"/>
+        <c:axId val="65725952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,12 +361,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58179584"/>
+        <c:crossAx val="66265088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58179584"/>
+        <c:axId val="66265088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +374,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80989568"/>
+        <c:crossAx val="65725952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -498,7 +392,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -737,114 +631,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$E$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Obj SoA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$B$23:$B$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>36000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>46000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>51000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$E$23:$E$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>13.056900000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89.471500000000006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>229.15299999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>436.09199999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>705.69600000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1037.94</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1427.39</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1907.47</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2456.67</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3070.84</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3756.39</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="48151168"/>
-        <c:axId val="48140288"/>
+        <c:axId val="66307200"/>
+        <c:axId val="66309120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48151168"/>
+        <c:axId val="66307200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,12 +660,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48140288"/>
+        <c:crossAx val="66309120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48140288"/>
+        <c:axId val="66309120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +673,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48151168"/>
+        <c:crossAx val="66307200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -900,7 +691,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1144,114 +935,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$E$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Obj SoA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$B$47:$B$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>36000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>46000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>51000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$E$47:$E$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>7.9457499999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.72158E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.8404500000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.3633800000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.6545699999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.2106100000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.7666600000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.12051099999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.15129999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.177786</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.201292</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="49181824"/>
-        <c:axId val="48168320"/>
+        <c:axId val="67850624"/>
+        <c:axId val="67852544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49181824"/>
+        <c:axId val="67850624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,12 +964,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48168320"/>
+        <c:crossAx val="67852544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48168320"/>
+        <c:axId val="67852544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +977,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49181824"/>
+        <c:crossAx val="67850624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1307,7 +995,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1695,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1707,21 +1395,18 @@
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -1734,9 +1419,7 @@
       <c r="D4" s="1">
         <v>10.303000000000001</v>
       </c>
-      <c r="E4" s="1">
-        <v>12.704599999999999</v>
-      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5">
       <c r="B5">
@@ -1748,9 +1431,6 @@
       <c r="D5">
         <v>41.444099999999999</v>
       </c>
-      <c r="E5">
-        <v>51.326300000000003</v>
-      </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6">
@@ -1762,9 +1442,6 @@
       <c r="D6">
         <v>93.022900000000007</v>
       </c>
-      <c r="E6">
-        <v>115.51300000000001</v>
-      </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7">
@@ -1776,9 +1453,6 @@
       <c r="D7">
         <v>165.78200000000001</v>
       </c>
-      <c r="E7">
-        <v>205.19</v>
-      </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8">
@@ -1790,9 +1464,6 @@
       <c r="D8">
         <v>257.67</v>
       </c>
-      <c r="E8">
-        <v>320.32400000000001</v>
-      </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9">
@@ -1804,9 +1475,6 @@
       <c r="D9">
         <v>374.51900000000001</v>
       </c>
-      <c r="E9">
-        <v>461.291</v>
-      </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10">
@@ -1818,9 +1486,6 @@
       <c r="D10">
         <v>508.423</v>
       </c>
-      <c r="E10">
-        <v>626.66600000000005</v>
-      </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11">
@@ -1832,9 +1497,6 @@
       <c r="D11">
         <v>662.68499999999995</v>
       </c>
-      <c r="E11">
-        <v>818.22900000000004</v>
-      </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12">
@@ -1846,9 +1508,6 @@
       <c r="D12">
         <v>837.37599999999998</v>
       </c>
-      <c r="E12">
-        <v>1034.8599999999999</v>
-      </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13">
@@ -1860,9 +1519,6 @@
       <c r="D13">
         <v>1031.6500000000001</v>
       </c>
-      <c r="E13">
-        <v>1276.76</v>
-      </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14">
@@ -1873,9 +1529,6 @@
       </c>
       <c r="D14">
         <v>1248.07</v>
-      </c>
-      <c r="E14">
-        <v>1542.46</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -1887,27 +1540,20 @@
         <f t="shared" ref="D15" si="0">SUM(D4:D14)</f>
         <v>5230.9450000000006</v>
       </c>
-      <c r="E15">
-        <f t="shared" ref="E15" si="1">SUM(E4:E14)</f>
-        <v>6465.3239000000003</v>
-      </c>
     </row>
     <row r="16" spans="2:5">
       <c r="D16" s="2">
         <f>(D15-$C15)/$C15</f>
         <v>7.9951740782728195E-2</v>
       </c>
-      <c r="E16" s="2">
-        <f>(E15-$C15)/$C15</f>
-        <v>0.33479472648425412</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1917,11 +1563,8 @@
       <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+    </row>
+    <row r="23" spans="2:4">
       <c r="B23">
         <v>1000</v>
       </c>
@@ -1931,11 +1574,8 @@
       <c r="D23">
         <v>12.1914</v>
       </c>
-      <c r="E23">
-        <v>13.056900000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
+    </row>
+    <row r="24" spans="2:4">
       <c r="B24">
         <v>6000</v>
       </c>
@@ -1945,11 +1585,8 @@
       <c r="D24">
         <v>82.227599999999995</v>
       </c>
-      <c r="E24">
-        <v>89.471500000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
+    </row>
+    <row r="25" spans="2:4">
       <c r="B25">
         <v>11000</v>
       </c>
@@ -1959,11 +1596,8 @@
       <c r="D25">
         <v>209.988</v>
       </c>
-      <c r="E25">
-        <v>229.15299999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
+    </row>
+    <row r="26" spans="2:4">
       <c r="B26">
         <v>16000</v>
       </c>
@@ -1973,11 +1607,8 @@
       <c r="D26">
         <v>395.99</v>
       </c>
-      <c r="E26">
-        <v>436.09199999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27">
         <v>21000</v>
       </c>
@@ -1987,11 +1618,8 @@
       <c r="D27">
         <v>642.077</v>
       </c>
-      <c r="E27">
-        <v>705.69600000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
+    </row>
+    <row r="28" spans="2:4">
       <c r="B28">
         <v>26000</v>
       </c>
@@ -2001,11 +1629,8 @@
       <c r="D28">
         <v>945.81100000000004</v>
       </c>
-      <c r="E28">
-        <v>1037.94</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
+    </row>
+    <row r="29" spans="2:4">
       <c r="B29">
         <v>31000</v>
       </c>
@@ -2015,11 +1640,8 @@
       <c r="D29">
         <v>1307.04</v>
       </c>
-      <c r="E29">
-        <v>1427.39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
+    </row>
+    <row r="30" spans="2:4">
       <c r="B30">
         <v>36000</v>
       </c>
@@ -2029,11 +1651,8 @@
       <c r="D30">
         <v>1739.69</v>
       </c>
-      <c r="E30">
-        <v>1907.47</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31">
         <v>41000</v>
       </c>
@@ -2043,11 +1662,8 @@
       <c r="D31">
         <v>2257.73</v>
       </c>
-      <c r="E31">
-        <v>2456.67</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
+    </row>
+    <row r="32" spans="2:4">
       <c r="B32">
         <v>46000</v>
       </c>
@@ -2056,9 +1672,6 @@
       </c>
       <c r="D32">
         <v>2880.59</v>
-      </c>
-      <c r="E32">
-        <v>3070.84</v>
       </c>
     </row>
     <row r="33" spans="2:5">
@@ -2070,9 +1683,6 @@
       </c>
       <c r="D33">
         <v>3645.97</v>
-      </c>
-      <c r="E33">
-        <v>3756.39</v>
       </c>
     </row>
     <row r="34" spans="2:5">
@@ -2081,12 +1691,8 @@
         <v>11290.9033</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:E34" si="2">SUM(D23:D33)</f>
+        <f t="shared" ref="D34:E34" si="1">SUM(D23:D33)</f>
         <v>14119.304999999998</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="2"/>
-        <v>15130.169399999999</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -2094,14 +1700,11 @@
         <f>(D34-$C34)/$C34</f>
         <v>0.25050269450097928</v>
       </c>
-      <c r="E35" s="2">
-        <f>(E34-$C34)/$C34</f>
-        <v>0.34003179355897939</v>
-      </c>
+      <c r="E35" s="2"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:5">
@@ -2114,9 +1717,6 @@
       <c r="D46" t="s">
         <v>2</v>
       </c>
-      <c r="E46" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47">
@@ -2128,9 +1728,6 @@
       <c r="D47">
         <v>8.0119700000000002E-2</v>
       </c>
-      <c r="E47">
-        <v>7.9457499999999997E-3</v>
-      </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48">
@@ -2142,9 +1739,6 @@
       <c r="D48">
         <v>0.49064999999999998</v>
       </c>
-      <c r="E48">
-        <v>1.72158E-2</v>
-      </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49">
@@ -2156,9 +1750,6 @@
       <c r="D49">
         <v>1.3117099999999999</v>
       </c>
-      <c r="E49">
-        <v>3.8404500000000001E-2</v>
-      </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50">
@@ -2170,9 +1761,6 @@
       <c r="D50">
         <v>2.48007</v>
       </c>
-      <c r="E50">
-        <v>5.3633800000000002E-2</v>
-      </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51">
@@ -2184,9 +1772,6 @@
       <c r="D51">
         <v>4.0632599999999996</v>
       </c>
-      <c r="E51">
-        <v>6.6545699999999999E-2</v>
-      </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52">
@@ -2198,9 +1783,6 @@
       <c r="D52">
         <v>5.9172700000000003</v>
       </c>
-      <c r="E52">
-        <v>8.2106100000000001E-2</v>
-      </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53">
@@ -2212,9 +1794,6 @@
       <c r="D53">
         <v>8.0801700000000007</v>
       </c>
-      <c r="E53">
-        <v>9.7666600000000006E-2</v>
-      </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54">
@@ -2226,9 +1805,6 @@
       <c r="D54">
         <v>10.545299999999999</v>
       </c>
-      <c r="E54">
-        <v>0.12051099999999999</v>
-      </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55">
@@ -2240,9 +1816,6 @@
       <c r="D55">
         <v>13.5594</v>
       </c>
-      <c r="E55">
-        <v>0.15129999999999999</v>
-      </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56">
@@ -2254,9 +1827,6 @@
       <c r="D56">
         <v>16.907900000000001</v>
       </c>
-      <c r="E56">
-        <v>0.177786</v>
-      </c>
     </row>
     <row r="57" spans="2:5">
       <c r="B57">
@@ -2267,9 +1837,6 @@
       </c>
       <c r="D57">
         <v>20.7242</v>
-      </c>
-      <c r="E57">
-        <v>0.201292</v>
       </c>
     </row>
     <row r="58" spans="2:5">
@@ -2278,12 +1845,8 @@
         <v>18.6298192</v>
       </c>
       <c r="D58">
-        <f t="shared" ref="D58" si="3">SUM(D47:D57)</f>
+        <f t="shared" ref="D58" si="2">SUM(D47:D57)</f>
         <v>84.160049699999988</v>
-      </c>
-      <c r="E58">
-        <f t="shared" ref="E58" si="4">SUM(E47:E57)</f>
-        <v>1.0144072499999999</v>
       </c>
     </row>
     <row r="59" spans="2:5">
@@ -2291,10 +1854,7 @@
         <f>(D58-$C58)/$C58</f>
         <v>3.517491490201901</v>
       </c>
-      <c r="E59" s="2">
-        <f>(E58-$C58)/$C58</f>
-        <v>-0.9455492702795526</v>
-      </c>
+      <c r="E59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>